<commit_message>
Database improvements + RES correction + Improved Outages
</commit_message>
<xml_diff>
--- a/Inputs/ARES_Africa/Annual_Generation_Statistics.xlsx
+++ b/Inputs/ARES_Africa/Annual_Generation_Statistics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\ARES_Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492D5CB4-54DF-4CF7-BB14-718CE9BA82F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AF9591-A745-4EE1-8768-93B19F0C3C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18900" windowHeight="11055" xr2:uid="{3016D1E9-EAE0-419D-90BD-C7C086BC9CE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3016D1E9-EAE0-419D-90BD-C7C086BC9CE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Generation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
         <v>25</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>165</v>
@@ -687,7 +687,7 @@
         <v>25</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <v>51</v>
@@ -791,7 +791,7 @@
         <v>25</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F10">
         <v>14970</v>
@@ -1057,7 +1057,7 @@
         <v>25</v>
       </c>
       <c r="E20">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F20">
         <v>431</v>

</xml_diff>